<commit_message>
updated Code for Maven
execute maven using pom.xml update are fixed
</commit_message>
<xml_diff>
--- a/CoreWorkStreamsTeam_B/ExcelFile/API_inputs.xlsx
+++ b/CoreWorkStreamsTeam_B/ExcelFile/API_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13425" windowHeight="6060" tabRatio="903" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13425" windowHeight="6060" tabRatio="903" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RLtoWOPMappingRule" sheetId="12" state="hidden" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="388">
   <si>
     <t>Content-Type</t>
   </si>
@@ -1292,6 +1292,15 @@
   </si>
   <si>
     <t>Campaign Test_1570</t>
+  </si>
+  <si>
+    <t>wocloud\nkumar</t>
+  </si>
+  <si>
+    <t>Amc@2727</t>
+  </si>
+  <si>
+    <t>Naresh</t>
   </si>
 </sst>
 </file>
@@ -2232,7 +2241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4654,10 +4663,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4700,10 +4709,22 @@
         <v>380</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C4" t="s">
+        <v>387</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Welcome@123"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>